<commit_message>
Change resonator to part with interchangeable pins
</commit_message>
<xml_diff>
--- a/Multi Edition/2.3B/SinESC-Multi-2.3B/Exported Files/BOM.xlsx
+++ b/Multi Edition/2.3B/SinESC-Multi-2.3B/Exported Files/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esamp\Documents\SinESC\Multi Edition\2.3B\SinESC-Multi-2.3B\Exported Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B6EA11-3C98-4BC0-B851-5F0BBC7FE233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5723D0D8-522B-4FCD-BB09-236F7661AA68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t>8MHz</t>
   </si>
   <si>
-    <t>CSTNE8M00GH5C000R0</t>
-  </si>
-  <si>
     <t>C1, C2, C4, C8, C17, C20, C30</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>BOM Consolidation Ratio (Total/Unique): 3.522</t>
+  </si>
+  <si>
+    <t>CSTNE8M00G550000R0</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1101,7 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1118,10 +1118,10 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1147,7 +1147,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1167,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5">
@@ -1188,10 +1188,10 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1208,10 +1208,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1291,7 +1291,7 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -1305,7 +1305,7 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>
@@ -1322,10 +1322,10 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
@@ -1339,10 +1339,10 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
         <v>22</v>
@@ -1356,10 +1356,10 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
         <v>23</v>
@@ -1373,10 +1373,10 @@
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
         <v>24</v>
@@ -1390,10 +1390,10 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" t="s">
         <v>25</v>
@@ -1407,10 +1407,10 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
@@ -1424,10 +1424,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H18" t="s">
         <v>27</v>
@@ -1441,10 +1441,10 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s">
         <v>28</v>
@@ -1461,7 +1461,7 @@
         <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
         <v>30</v>
@@ -1492,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
@@ -1549,7 +1549,7 @@
         <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change total component count to correct value of 75, recalculate BOM Consolidation Ratio
</commit_message>
<xml_diff>
--- a/Multi Edition/2.3B/SinESC-Multi-2.3B/Exported Files/BOM.xlsx
+++ b/Multi Edition/2.3B/SinESC-Multi-2.3B/Exported Files/BOM.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esamp\Documents\SinESC\Multi Edition\2.3B\SinESC-Multi-2.3B\Exported Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5723D0D8-522B-4FCD-BB09-236F7661AA68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119782DA-52E5-4A5B-A3B5-40AEF1217737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="78">
   <si>
     <t>Qty</t>
   </si>
@@ -190,12 +200,6 @@
     <t>U2, U3, U5</t>
   </si>
   <si>
-    <t>SinESC Multi v2.3B</t>
-  </si>
-  <si>
-    <t>Bill of Materials (BOM)</t>
-  </si>
-  <si>
     <t>Source: SinESC\Multi Edition\2.3B\SinESC-Multi-2.3B\SinESC-Multi-2.3B.sch</t>
   </si>
   <si>
@@ -208,9 +212,6 @@
     <t>Generator: bom_csv_grouped_by_value.py</t>
   </si>
   <si>
-    <t>Total Component Count: 81</t>
-  </si>
-  <si>
     <t>1µF</t>
   </si>
   <si>
@@ -253,10 +254,16 @@
     <t>Unique Component Count: 23</t>
   </si>
   <si>
-    <t>BOM Consolidation Ratio (Total/Unique): 3.522</t>
-  </si>
-  <si>
     <t>CSTNE8M00G550000R0</t>
+  </si>
+  <si>
+    <t>Total Component Count: 75</t>
+  </si>
+  <si>
+    <t>BOM Consolidation Ratio (Total/Unique): 3.261</t>
+  </si>
+  <si>
+    <t>SinESC Multi v2.3B - Bill of Materials (BOM)</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1108,7 @@
   <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1118,10 +1125,10 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -1138,7 +1145,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1158,7 +1165,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1178,7 +1185,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5">
@@ -1191,7 +1198,7 @@
         <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H5" t="s">
         <v>8</v>
@@ -1199,7 +1206,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1211,7 +1218,7 @@
         <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
@@ -1219,7 +1226,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1239,7 +1246,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1278,9 +1285,6 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
       <c r="D10">
         <v>8</v>
       </c>
@@ -1291,7 +1295,7 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -1325,7 +1329,7 @@
         <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
         <v>21</v>
@@ -1342,7 +1346,7 @@
         <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
         <v>22</v>
@@ -1359,7 +1363,7 @@
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
         <v>23</v>
@@ -1376,7 +1380,7 @@
         <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
         <v>24</v>
@@ -1393,7 +1397,7 @@
         <v>51</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H16" t="s">
         <v>25</v>
@@ -1410,7 +1414,7 @@
         <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
@@ -1427,7 +1431,7 @@
         <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
         <v>27</v>
@@ -1444,7 +1448,7 @@
         <v>54</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H19" t="s">
         <v>28</v>
@@ -1461,7 +1465,7 @@
         <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
         <v>30</v>
@@ -1549,7 +1553,7 @@
         <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>